<commit_message>
added ReadAndWriteRanges and new version of SimpleModel.xlsx
</commit_message>
<xml_diff>
--- a/SimpleModel.xlsx
+++ b/SimpleModel.xlsx
@@ -4,18 +4,22 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="model_sheet_1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="model_sheet_2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="input.data">model_sheet_2!$C$3:$C$12</definedName>
+    <definedName name="output.data">model_sheet_2!$C$17:$C$26</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>&lt;set the value in cell A1 from R</t>
   </si>
@@ -24,14 +28,94 @@
   </si>
   <si>
     <t>&lt;perform some calculations</t>
+  </si>
+  <si>
+    <t>inputs:</t>
+  </si>
+  <si>
+    <t>outputs:</t>
+  </si>
+  <si>
+    <t>input_1</t>
+  </si>
+  <si>
+    <t>input_2</t>
+  </si>
+  <si>
+    <t>input_3</t>
+  </si>
+  <si>
+    <t>input_4</t>
+  </si>
+  <si>
+    <t>input_5</t>
+  </si>
+  <si>
+    <t>input_6</t>
+  </si>
+  <si>
+    <t>input_7</t>
+  </si>
+  <si>
+    <t>input_8</t>
+  </si>
+  <si>
+    <t>input_9</t>
+  </si>
+  <si>
+    <t>input_10</t>
+  </si>
+  <si>
+    <t>output_1</t>
+  </si>
+  <si>
+    <t>output_2</t>
+  </si>
+  <si>
+    <t>output_3</t>
+  </si>
+  <si>
+    <t>output_4</t>
+  </si>
+  <si>
+    <t>output_5</t>
+  </si>
+  <si>
+    <t>output_6</t>
+  </si>
+  <si>
+    <t>output_7</t>
+  </si>
+  <si>
+    <t>output_8</t>
+  </si>
+  <si>
+    <t>output_9</t>
+  </si>
+  <si>
+    <t>output_10</t>
+  </si>
+  <si>
+    <t>Methodology:</t>
+  </si>
+  <si>
+    <t>random input data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -47,7 +131,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -55,12 +139,53 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -357,7 +482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -372,7 +497,7 @@
       </c>
       <c r="H1" t="str">
         <f ca="1">CELL("filename")</f>
-        <v>C:\Users\DECC\Documents\R_Greg\Excel_link_to_R\[SimpleModel.xlsx]model_sheet_1</v>
+        <v>C:\Users\DECC\Documents\R_Excel_link\[SimpleModel.xlsx]model_sheet_2</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -409,12 +534,279 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="B2:K26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11">
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" t="str">
+        <f ca="1">CELL("filename")</f>
+        <v>C:\Users\DECC\Documents\R_Excel_link\[SimpleModel.xlsx]model_sheet_2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <f>C3*300</f>
+        <v>300</v>
+      </c>
+      <c r="I3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11">
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <f>F3/C4</f>
+        <v>150</v>
+      </c>
+      <c r="K4">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <f>SUM(F3:F4)/C5</f>
+        <v>150</v>
+      </c>
+      <c r="K5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <f>F5+C6</f>
+        <v>154</v>
+      </c>
+      <c r="K6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11">
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <f>F6+C7*C8</f>
+        <v>184</v>
+      </c>
+      <c r="K7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11">
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <f>F7/C8</f>
+        <v>30.666666666666668</v>
+      </c>
+      <c r="K8">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11">
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="2">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <f>F8+C9</f>
+        <v>37.666666666666671</v>
+      </c>
+      <c r="K9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11">
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="2">
+        <v>8</v>
+      </c>
+      <c r="F10">
+        <f>F9/C10*C9</f>
+        <v>32.958333333333336</v>
+      </c>
+      <c r="K10">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11">
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="2">
+        <v>9</v>
+      </c>
+      <c r="F11">
+        <f>F10-C11</f>
+        <v>23.958333333333336</v>
+      </c>
+      <c r="K11">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11">
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="3">
+        <v>10</v>
+      </c>
+      <c r="F12">
+        <f>F11/C12</f>
+        <v>2.3958333333333335</v>
+      </c>
+      <c r="K12">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11">
+      <c r="C16" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="1">
+        <f>F3</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="2">
+        <f t="shared" ref="C18:C26" si="0">F4</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="2">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="2">
+        <f t="shared" si="0"/>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3">
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="2">
+        <f t="shared" si="0"/>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="2">
+        <f t="shared" si="0"/>
+        <v>30.666666666666668</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3">
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="2">
+        <f t="shared" si="0"/>
+        <v>37.666666666666671</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3">
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="2">
+        <f t="shared" si="0"/>
+        <v>32.958333333333336</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3">
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="2">
+        <f t="shared" si="0"/>
+        <v>23.958333333333336</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3">
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="3">
+        <f t="shared" si="0"/>
+        <v>2.3958333333333335</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added V2 of montecarlo.r, which calculates the results in the model rather than in R
</commit_message>
<xml_diff>
--- a/SimpleModel.xlsx
+++ b/SimpleModel.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>&lt;set the value in cell A1 from R</t>
   </si>
@@ -122,6 +122,12 @@
   </si>
   <si>
     <t>total saving</t>
+  </si>
+  <si>
+    <t>Chosen</t>
+  </si>
+  <si>
+    <t>per unit savings</t>
   </si>
 </sst>
 </file>
@@ -214,13 +220,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -533,7 +542,7 @@
       </c>
       <c r="H1" t="str">
         <f ca="1">CELL("filename")</f>
-        <v>C:\Users\DECC\Documents\R_Greg\R_Excel_link\[SimpleModel.xlsx]mc_model</v>
+        <v>C:\Users\DECC\Documents\GitHub\R_Excel_link\[SimpleModel.xlsx]mc_model</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -573,7 +582,7 @@
   <dimension ref="B2:K26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -590,7 +599,7 @@
       </c>
       <c r="I2" t="str">
         <f ca="1">CELL("filename")</f>
-        <v>C:\Users\DECC\Documents\R_Greg\R_Excel_link\[SimpleModel.xlsx]mc_model</v>
+        <v>C:\Users\DECC\Documents\GitHub\R_Excel_link\[SimpleModel.xlsx]mc_model</v>
       </c>
     </row>
     <row r="3" spans="2:11">
@@ -849,10 +858,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:D10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -862,21 +871,27 @@
     <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4">
+    <row r="1" spans="1:6">
       <c r="D1" t="str">
         <f ca="1">CELL("filename")</f>
-        <v>C:\Users\DECC\Documents\R_Greg\R_Excel_link\[SimpleModel.xlsx]mc_model</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4">
+        <v>C:\Users\DECC\Documents\GitHub\R_Excel_link\[SimpleModel.xlsx]mc_model</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="C3" t="s">
         <v>31</v>
       </c>
       <c r="D3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="2:4">
+      <c r="F3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="6" t="s">
+        <v>35</v>
+      </c>
       <c r="B4" t="s">
         <v>27</v>
       </c>
@@ -886,8 +901,12 @@
       <c r="D4">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="2:4">
+      <c r="F4">
+        <v>13.326968561774708</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="6"/>
       <c r="B5" t="s">
         <v>28</v>
       </c>
@@ -897,8 +916,12 @@
       <c r="D5">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="2:4">
+      <c r="F5">
+        <v>2.5902509112174479</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="6"/>
       <c r="B6" t="s">
         <v>29</v>
       </c>
@@ -908,8 +931,11 @@
       <c r="D6">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="2:4">
+      <c r="F6">
+        <v>5.9287237927946732</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="B7" t="s">
         <v>30</v>
       </c>
@@ -919,8 +945,11 @@
       <c r="D7" s="5">
         <v>35000</v>
       </c>
-    </row>
-    <row r="10" spans="2:4">
+      <c r="F7">
+        <v>16888.885371193061</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="B10" t="s">
         <v>33</v>
       </c>
@@ -932,8 +961,15 @@
         <f>SUM(D4:D6)*D7</f>
         <v>1295000</v>
       </c>
+      <c r="F10" s="5">
+        <f>SUM(F4:F6)*F7</f>
+        <v>368953.63164146076</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A4:A6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added Simple_Example.R and example.xlsx
</commit_message>
<xml_diff>
--- a/SimpleModel.xlsx
+++ b/SimpleModel.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>&lt;set the value in cell A1 from R</t>
   </si>
@@ -124,13 +124,52 @@
     <t>Chosen</t>
   </si>
   <si>
-    <t>per unit savings</t>
-  </si>
-  <si>
     <t>total saving per unit:</t>
   </si>
   <si>
-    <t>Total overall saving:</t>
+    <t>Total  saving:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">per unit savings </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(£ 95% confident)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Is it worth investing </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>£400,000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in a new machine?</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -141,7 +180,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,6 +198,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -185,7 +247,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -245,30 +307,83 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="1" tint="0.499984740745262"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom style="thick">
+        <color theme="1" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top style="thick">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom style="thick">
+        <color theme="1" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -897,123 +1012,182 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F10"/>
+  <dimension ref="C1:S12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5"/>
-    <col min="2" max="2" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="5" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="2" width="9.140625" style="5"/>
+    <col min="3" max="3" width="22.140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="29.5703125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="17" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6" style="5" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" style="5" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" style="5" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="D1" s="5" t="str">
+    <row r="1" spans="3:19">
+      <c r="S1" s="5" t="str">
         <f ca="1">CELL("filename")</f>
         <v>C:\Users\DECC\Documents\GitHub\R_Excel_link\[SimpleModel.xlsx]mc_model</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="C3" s="6" t="s">
+    <row r="2" spans="3:19" ht="26.25">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="3:19" ht="26.25">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="3:19" ht="26.25">
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="F4" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="G4" s="16"/>
+      <c r="H4" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="13" t="s">
+    <row r="5" spans="3:19" ht="26.25">
+      <c r="C5" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="9">
+        <v>10</v>
+      </c>
+      <c r="F5" s="9">
+        <v>20</v>
+      </c>
+      <c r="G5" s="17"/>
+      <c r="H5" s="12">
+        <v>17.069124950116777</v>
+      </c>
+    </row>
+    <row r="6" spans="3:19" ht="26.25">
+      <c r="C6" s="21"/>
+      <c r="D6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="9">
+        <v>-2</v>
+      </c>
+      <c r="F6" s="9">
+        <v>8</v>
+      </c>
+      <c r="G6" s="17"/>
+      <c r="H6" s="12">
+        <v>2.2016810373342999</v>
+      </c>
+    </row>
+    <row r="7" spans="3:19" ht="26.25">
+      <c r="C7" s="21"/>
+      <c r="D7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="9">
+        <v>3</v>
+      </c>
+      <c r="F7" s="9">
+        <v>9</v>
+      </c>
+      <c r="G7" s="17"/>
+      <c r="H7" s="12">
+        <v>1.9144548097642353</v>
+      </c>
+    </row>
+    <row r="8" spans="3:19" ht="26.25">
+      <c r="C8" s="14"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="12"/>
+    </row>
+    <row r="9" spans="3:19" ht="26.25">
+      <c r="C9" s="6"/>
+      <c r="D9" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="10">
+        <v>15000</v>
+      </c>
+      <c r="F9" s="10">
+        <v>35000</v>
+      </c>
+      <c r="G9" s="18"/>
+      <c r="H9" s="11">
+        <v>33602.907905897053</v>
+      </c>
+    </row>
+    <row r="10" spans="3:19" ht="27" thickBot="1">
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="3:19" ht="54" thickTop="1" thickBot="1">
+      <c r="C11" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="7">
-        <v>10</v>
-      </c>
-      <c r="D4" s="7">
-        <v>20</v>
-      </c>
-      <c r="F4" s="5">
-        <v>14.54093161873365</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="13"/>
-      <c r="B5" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="7">
-        <v>-2</v>
-      </c>
-      <c r="D5" s="7">
-        <v>8</v>
-      </c>
-      <c r="F5" s="5">
-        <v>1.326968561774708</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="13"/>
-      <c r="B6" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="7">
-        <v>3</v>
-      </c>
-      <c r="D6" s="7">
-        <v>9</v>
-      </c>
-      <c r="F6" s="5">
-        <v>5.754150546730469</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="B7" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="8">
-        <v>15000</v>
-      </c>
-      <c r="D7" s="8">
-        <v>35000</v>
-      </c>
-      <c r="F7" s="5">
-        <v>24762.412642648909</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="45">
-      <c r="B10" s="10" t="s">
+      <c r="D11" s="23"/>
+      <c r="E11" s="13">
+        <f>SUM(E5:E7)*E9</f>
+        <v>165000</v>
+      </c>
+      <c r="F11" s="13">
+        <f>SUM(F5:F7)*F9</f>
+        <v>1295000</v>
+      </c>
+      <c r="G11" s="13"/>
+      <c r="H11" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="9">
-        <f>SUM(C4:C6)*C7</f>
-        <v>165000</v>
-      </c>
-      <c r="D10" s="9">
-        <f>SUM(D4:D6)*D7</f>
-        <v>1295000</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="11">
-        <f>SUM(F4:F6)*F7</f>
-        <v>535414.14228817471</v>
-      </c>
+      <c r="I11" s="20">
+        <f>SUM(H5:H7)*H9</f>
+        <v>711886.36753123731</v>
+      </c>
+    </row>
+    <row r="12" spans="3:19" ht="27" thickTop="1">
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A4:A6"/>
+  <mergeCells count="2">
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>